<commit_message>
Initial Glider Design v5.0
- Python
- Integrate roll-in kinematic model
</commit_message>
<xml_diff>
--- a/01_Initial_Glider_Design/results/nausicaa_results.xlsx
+++ b/01_Initial_Glider_Design/results/nausicaa_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B171"/>
+  <dimension ref="A1:B175"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5.153149587064384</v>
+        <v>5.15314950125791</v>
       </c>
     </row>
     <row r="3">
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>10.00000000236661</v>
+        <v>10.0000000023666</v>
       </c>
     </row>
     <row r="4">
@@ -472,7 +472,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>64.99999959370463</v>
+        <v>64.99999959370513</v>
       </c>
     </row>
     <row r="5">
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1.262260661268573</v>
+        <v>1.262260619232062</v>
       </c>
     </row>
     <row r="6">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2.36620154716941</v>
+        <v>2.366201547169455</v>
       </c>
     </row>
     <row r="7">
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.0811950322550842</v>
+        <v>0.08119500858660114</v>
       </c>
     </row>
     <row r="8">
@@ -512,7 +512,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>8.789210090588769</v>
+        <v>8.789208473547559</v>
       </c>
     </row>
     <row r="9">
@@ -522,7 +522,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1.387313579584675</v>
+        <v>1.38731381172129</v>
       </c>
     </row>
     <row r="10">
@@ -532,7 +532,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1.386476893843071</v>
+        <v>1.386477125956847</v>
       </c>
     </row>
     <row r="11">
@@ -542,7 +542,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-0.0008366857416042262</v>
+        <v>-0.000836685764442846</v>
       </c>
     </row>
     <row r="12">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.04000007392751177</v>
+        <v>0.04000007495289409</v>
       </c>
     </row>
     <row r="13">
@@ -562,7 +562,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.4000000353818571</v>
+        <v>0.4000000353914301</v>
       </c>
     </row>
     <row r="14">
@@ -572,7 +572,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.01999999266704567</v>
+        <v>0.01999999266748676</v>
       </c>
     </row>
     <row r="15">
@@ -582,7 +582,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>49656.65253802875</v>
+        <v>49656.64906183934</v>
       </c>
     </row>
     <row r="16">
@@ -592,7 +592,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-0.09342456682821094</v>
+        <v>-0.09342432032415242</v>
       </c>
     </row>
     <row r="17">
@@ -602,7 +602,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.696832722207728</v>
+        <v>0.6968314948820026</v>
       </c>
     </row>
     <row r="18">
@@ -612,7 +612,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.7948884506379511</v>
+        <v>0.7948882740313044</v>
       </c>
     </row>
     <row r="19">
@@ -622,7 +622,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>2.035398503147315</v>
+        <v>2.035398188995389</v>
       </c>
     </row>
     <row r="20">
@@ -632,7 +632,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.1407575007310229</v>
+        <v>0.1407574932211545</v>
       </c>
     </row>
     <row r="21">
@@ -652,7 +652,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.1118865116717531</v>
+        <v>0.1118864808435365</v>
       </c>
     </row>
     <row r="23">
@@ -662,7 +662,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.696832722207728</v>
+        <v>0.6968314948820026</v>
       </c>
     </row>
     <row r="24">
@@ -672,7 +672,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.1901605316065426</v>
+        <v>0.1901606678026856</v>
       </c>
     </row>
     <row r="25">
@@ -682,7 +682,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.04754013290163565</v>
+        <v>0.0475401669506714</v>
       </c>
     </row>
     <row r="26">
@@ -702,7 +702,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.009040256945220721</v>
+        <v>0.009040269894790839</v>
       </c>
     </row>
     <row r="28">
@@ -712,7 +712,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.696832722207728</v>
+        <v>0.6968314948820026</v>
       </c>
     </row>
     <row r="29">
@@ -722,7 +722,7 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.07145088433007531</v>
+        <v>0.07145092947298221</v>
       </c>
     </row>
     <row r="30">
@@ -732,7 +732,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.03572544216503765</v>
+        <v>0.0357254647364911</v>
       </c>
     </row>
     <row r="31">
@@ -752,7 +752,7 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0.0025526144357749</v>
+        <v>0.002552617661276538</v>
       </c>
     </row>
     <row r="33">
@@ -792,7 +792,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>1.621983713667576e-15</v>
+        <v>2.089214277619248e-16</v>
       </c>
     </row>
     <row r="37">
@@ -802,7 +802,7 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>-1.735103943716778e-14</v>
+        <v>-2.055181882769011e-14</v>
       </c>
     </row>
     <row r="38">
@@ -812,393 +812,393 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>-3.026542488249412</v>
+        <v>-3.026541759043032</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>objective_total</t>
+          <t>p_roll (rad/s)</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>0.01065729830310768</v>
+        <v>1.129190841214659</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>objective_sink</t>
+          <t>p_roll (deg/s)</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>0</v>
+        <v>64.69786946642702</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>objective_climb</t>
+          <t>t_roll (s)</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>7.000430302038139e-07</v>
+        <v>1.004669862080001</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>objective_mass</t>
+          <t>psi_0 (deg)</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>0</v>
+        <v>-14.37798939844673</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>objective_span</t>
+          <t>objective_total</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>0.01056499866574569</v>
+        <v>0.01065729830633046</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>objective_control</t>
+          <t>objective_sink</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>9.159959433178941e-05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>penalty</t>
+          <t>objective_climb</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>8.55534373972331e-11</v>
+        <v>7.000430684213097e-07</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>x_cg (m)</t>
+          <t>objective_mass</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>0.02675086760233792</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>y_cg (m)</t>
+          <t>objective_span</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>1.366991125785201e-18</v>
+        <v>0.01056499871306972</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>z_cg (m)</t>
+          <t>objective_control</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>0.00311316553197908</v>
+        <v>9.159955019231291e-05</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>I_xx (kg m^2)</t>
+          <t>penalty</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>0.001835682493587644</v>
+        <v>1.79408783147668e-13</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>I_yy (kg m^2)</t>
+          <t>x_cg (m)</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>0.001454773590881659</v>
+        <v>0.02675087597365176</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>I_zz (kg m^2)</t>
+          <t>y_cg (m)</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>0.003286804395816139</v>
+        <v>7.254640258807773e-18</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>I_xy (kg m^2)</t>
+          <t>z_cg (m)</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>3.002170370927886e-21</v>
+        <v>0.003113164496971128</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>I_xz (kg m^2)</t>
+          <t>I_xx (kg m^2)</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>-6.229708233294081e-06</v>
+        <v>0.001835681086377205</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>I_yz (kg m^2)</t>
+          <t>I_yy (kg m^2)</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>1.34931540360727e-21</v>
+        <v>0.001454767579799796</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>mass_wing_kg</t>
+          <t>I_zz (kg m^2)</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>0.03232608428599095</v>
+        <v>0.003286796979129735</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>mass_htail_surfaces_kg</t>
+          <t>I_xy (kg m^2)</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>0.0007772678986920224</v>
+        <v>-7.012946177065933e-21</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>mass_vtail_surfaces_kg</t>
+          <t>I_xz (kg m^2)</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>0.0001649272431053734</v>
+        <v>-6.229706794991583e-06</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>mass_linkages_kg</t>
+          <t>I_yz (kg m^2)</t>
         </is>
       </c>
       <c r="B58" t="n">
-        <v>0.001</v>
+        <v>-3.216441650377974e-21</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>mass_Receiver_kg</t>
+          <t>mass_wing_kg</t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>0.005</v>
+        <v>0.03232607365444774</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>mass_battery_kg</t>
+          <t>mass_htail_surfaces_kg</t>
         </is>
       </c>
       <c r="B60" t="n">
-        <v>0.013</v>
+        <v>0.0007772695687699006</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>mass_servo_kg</t>
+          <t>mass_vtail_surfaces_kg</t>
         </is>
       </c>
       <c r="B61" t="n">
-        <v>0.008800000000000001</v>
+        <v>0.0001649275557103168</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>mass_boom_kg</t>
+          <t>mass_linkages_kg</t>
         </is>
       </c>
       <c r="B62" t="n">
-        <v>0.00711231560132345</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>mass_pod_kg</t>
+          <t>mass_Receiver_kg</t>
         </is>
       </c>
       <c r="B63" t="n">
-        <v>0.007</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>mass_ballast_kg</t>
+          <t>mass_battery_kg</t>
         </is>
       </c>
       <c r="B64" t="n">
-        <v>-9.60773753408204e-09</v>
+        <v>0.013</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>mass_glue_weight_kg</t>
+          <t>mass_servo_kg</t>
         </is>
       </c>
       <c r="B65" t="n">
-        <v>0.006014446833709941</v>
+        <v>0.008800000000000001</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>wing root LE x (m)</t>
+          <t>mass_boom_kg</t>
         </is>
       </c>
       <c r="B66" t="n">
-        <v>-0.03518937518275572</v>
+        <v>0.007112302336855394</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>wing root LE y (m)</t>
+          <t>mass_pod_kg</t>
         </is>
       </c>
       <c r="B67" t="n">
-        <v>0</v>
+        <v>0.007</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>wing root LE z (m)</t>
+          <t>mass_ballast_kg</t>
         </is>
       </c>
       <c r="B68" t="n">
-        <v>0</v>
+        <v>-9.609671186080976e-09</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>wing tip LE x (m)</t>
+          <t>mass_glue_weight_kg</t>
         </is>
       </c>
       <c r="B69" t="n">
-        <v>-0.03518937518275572</v>
+        <v>0.006014445080488974</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>wing tip LE y (m)</t>
+          <t>wing root LE x (m)</t>
         </is>
       </c>
       <c r="B70" t="n">
-        <v>0.3971934676874264</v>
+        <v>-0.03518937330528862</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>wing tip LE z (m)</t>
+          <t>wing root LE y (m)</t>
         </is>
       </c>
       <c r="B71" t="n">
-        <v>0.01411600034846825</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>htail root LE x (m)</t>
+          <t>wing root LE z (m)</t>
         </is>
       </c>
       <c r="B72" t="n">
-        <v>0.6492925893060923</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>htail root LE y (m)</t>
+          <t>wing tip LE x (m)</t>
         </is>
       </c>
       <c r="B73" t="n">
-        <v>0</v>
+        <v>-0.03518937330528862</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>htail root LE z (m)</t>
+          <t>wing tip LE y (m)</t>
         </is>
       </c>
       <c r="B74" t="n">
-        <v>0</v>
+        <v>0.3971933795172136</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>htail tip LE x (m)</t>
+          <t>wing tip LE z (m)</t>
         </is>
       </c>
       <c r="B75" t="n">
-        <v>0.6492925893060923</v>
+        <v>0.01411599503439941</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>htail tip LE y (m)</t>
+          <t>htail root LE x (m)</t>
         </is>
       </c>
       <c r="B76" t="n">
-        <v>0.09508026580327129</v>
+        <v>0.6492913279313312</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>htail tip LE z (m)</t>
+          <t>htail root LE y (m)</t>
         </is>
       </c>
       <c r="B77" t="n">
@@ -1208,941 +1208,981 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>vtail root LE x (m)</t>
+          <t>htail root LE z (m)</t>
         </is>
       </c>
       <c r="B78" t="n">
-        <v>0.6611072800426903</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>vtail root LE y (m)</t>
+          <t>htail tip LE x (m)</t>
         </is>
       </c>
       <c r="B79" t="n">
-        <v>0</v>
+        <v>0.6492913279313312</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>vtail root LE z (m)</t>
+          <t>htail tip LE y (m)</t>
         </is>
       </c>
       <c r="B80" t="n">
-        <v>0</v>
+        <v>0.09508033390134281</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>vtail tip LE x (m)</t>
+          <t>htail tip LE z (m)</t>
         </is>
       </c>
       <c r="B81" t="n">
-        <v>0.6611072800426903</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>vtail tip LE y (m)</t>
+          <t>vtail root LE x (m)</t>
         </is>
       </c>
       <c r="B82" t="n">
-        <v>0</v>
+        <v>0.6611060301455115</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>vtail tip LE z (m)</t>
+          <t>vtail root LE y (m)</t>
         </is>
       </c>
       <c r="B83" t="n">
-        <v>0.07145088433007531</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>aero_F_g[0]</t>
+          <t>vtail root LE z (m)</t>
         </is>
       </c>
       <c r="B84" t="n">
-        <v>-0.1161011988132716</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>aero_F_g[1]</t>
+          <t>vtail tip LE x (m)</t>
         </is>
       </c>
       <c r="B85" t="n">
-        <v>3.847629485179784e-17</v>
+        <v>0.6611060301455115</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>aero_F_g[2]</t>
+          <t>vtail tip LE y (m)</t>
         </is>
       </c>
       <c r="B86" t="n">
-        <v>1.89333787841236</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>aero_M_g[0]</t>
+          <t>vtail tip LE z (m)</t>
         </is>
       </c>
       <c r="B87" t="n">
-        <v>-1.311885011390024e-18</v>
+        <v>0.07145092947298221</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>aero_M_g[1]</t>
+          <t>aero_F_g[0]</t>
         </is>
       </c>
       <c r="B88" t="n">
-        <v>2.730521798249841e-10</v>
+        <v>-0.1161011261167751</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>aero_M_g[2]</t>
+          <t>aero_F_g[1]</t>
         </is>
       </c>
       <c r="B89" t="n">
-        <v>2.466429218667608e-17</v>
+        <v>4.424779351762667e-17</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>aero_F_b</t>
+          <t>aero_F_g[2]</t>
         </is>
       </c>
       <c r="B90" t="n">
-        <v>0.1161011988132716</v>
+        <v>1.893337333351328</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>aero_F_w</t>
+          <t>aero_M_g[0]</t>
         </is>
       </c>
       <c r="B91" t="n">
-        <v>-0.2144373116466061</v>
+        <v>-1.907679116775153e-18</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>aero_M_b</t>
+          <t>aero_M_g[1]</t>
         </is>
       </c>
       <c r="B92" t="n">
-        <v>1.311885011390024e-18</v>
+        <v>7.43762690325056e-17</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>aero_M_w</t>
+          <t>aero_M_g[2]</t>
         </is>
       </c>
       <c r="B93" t="n">
-        <v>-2.9909548623963e-18</v>
+        <v>2.741624099008162e-17</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>aero_L</t>
+          <t>aero_F_b</t>
         </is>
       </c>
       <c r="B94" t="n">
-        <v>1.88473458332219</v>
+        <v>0.1161011261167751</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>aero_Y</t>
+          <t>aero_F_w</t>
         </is>
       </c>
       <c r="B95" t="n">
-        <v>3.847629485179784e-17</v>
+        <v>-0.2144372885898241</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>aero_D</t>
+          <t>aero_M_b</t>
         </is>
       </c>
       <c r="B96" t="n">
-        <v>0.2144373116466061</v>
+        <v>1.907679116775153e-18</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>aero_l_b</t>
+          <t>aero_M_w</t>
         </is>
       </c>
       <c r="B97" t="n">
-        <v>1.311885011390024e-18</v>
+        <v>-2.882083103074324e-18</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>aero_m_b</t>
+          <t>aero_L</t>
         </is>
       </c>
       <c r="B98" t="n">
-        <v>2.730521798249841e-10</v>
+        <v>1.884734033918247</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>aero_n_b</t>
+          <t>aero_Y</t>
         </is>
       </c>
       <c r="B99" t="n">
-        <v>-2.466429218667608e-17</v>
+        <v>4.424779351762667e-17</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>aero_CL</t>
+          <t>aero_D</t>
         </is>
       </c>
       <c r="B100" t="n">
-        <v>1.0356694673591</v>
+        <v>0.2144372885898241</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>aero_CY</t>
+          <t>aero_l_b</t>
         </is>
       </c>
       <c r="B101" t="n">
-        <v>2.114288353794223e-17</v>
+        <v>1.907679116775153e-18</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>aero_CD</t>
+          <t>aero_m_b</t>
         </is>
       </c>
       <c r="B102" t="n">
-        <v>0.1178341917743613</v>
+        <v>7.43762690325056e-17</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>aero_Cl</t>
+          <t>aero_n_b</t>
         </is>
       </c>
       <c r="B103" t="n">
-        <v>9.069024113464289e-19</v>
+        <v>-2.741624099008162e-17</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>aero_Cm</t>
+          <t>aero_CL</t>
         </is>
       </c>
       <c r="B104" t="n">
-        <v>1.065970225867037e-09</v>
+        <v>1.035669485308945</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>aero_Cn</t>
+          <t>aero_CY</t>
         </is>
       </c>
       <c r="B105" t="n">
-        <v>-1.705035568212569e-17</v>
+        <v>2.431435349166336e-17</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>wing_components_comp1_L (N)</t>
+          <t>aero_CD</t>
         </is>
       </c>
       <c r="B106" t="n">
-        <v>1.82076627889601</v>
+        <v>0.1178342154957352</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>wing_components_comp1_D (N)</t>
+          <t>aero_Cl</t>
         </is>
       </c>
       <c r="B107" t="n">
-        <v>0.06728618149527207</v>
+        <v>1.318773897673912e-18</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>wing_components_comp1_Y (N)</t>
+          <t>aero_Cm</t>
         </is>
       </c>
       <c r="B108" t="n">
-        <v>0</v>
+        <v>2.903581178724765e-16</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>wing_components_comp1_l_b</t>
+          <t>aero_Cn</t>
         </is>
       </c>
       <c r="B109" t="n">
-        <v>-0</v>
+        <v>-1.895278019878785e-17</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>wing_components_comp1_m_b</t>
+          <t>wing_components_comp1_L (N)</t>
         </is>
       </c>
       <c r="B110" t="n">
-        <v>0.0402413425085334</v>
+        <v>1.82076560353693</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>wing_components_comp1_n_b</t>
+          <t>wing_components_comp1_D (N)</t>
         </is>
       </c>
       <c r="B111" t="n">
-        <v>-0</v>
+        <v>0.06728616654041117</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>wing_components_comp1_span_eff (m)</t>
+          <t>wing_components_comp1_Y (N)</t>
         </is>
       </c>
       <c r="B112" t="n">
-        <v>0.7943870935841959</v>
+        <v>0</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>wing_components_comp1_oswald</t>
+          <t>wing_components_comp1_l_b</t>
         </is>
       </c>
       <c r="B113" t="n">
-        <v>0.8006279876453991</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>wing_components_comp2_L (N)</t>
+          <t>wing_components_comp1_m_b</t>
         </is>
       </c>
       <c r="B114" t="n">
-        <v>0.06228084168136074</v>
+        <v>0.04024134289077547</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>wing_components_comp2_D (N)</t>
+          <t>wing_components_comp1_n_b</t>
         </is>
       </c>
       <c r="B115" t="n">
-        <v>0.007013510299280108</v>
+        <v>8.673617379884035e-19</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>wing_components_comp2_Y (N)</t>
+          <t>wing_components_comp1_span_eff (m)</t>
         </is>
       </c>
       <c r="B116" t="n">
-        <v>0</v>
+        <v>0.7943869172436374</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>wing_components_comp2_l_b</t>
+          <t>wing_components_comp1_oswald</t>
         </is>
       </c>
       <c r="B117" t="n">
-        <v>5.421010862427522e-20</v>
+        <v>0.8006279933964573</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>wing_components_comp2_m_b</t>
+          <t>wing_components_comp2_L (N)</t>
         </is>
       </c>
       <c r="B118" t="n">
-        <v>-0.03964930110115668</v>
+        <v>0.06228097086874435</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>wing_components_comp2_n_b</t>
+          <t>wing_components_comp2_D (N)</t>
         </is>
       </c>
       <c r="B119" t="n">
-        <v>3.388131789017201e-21</v>
+        <v>0.0070135186718487</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>wing_components_comp2_span_eff (m)</t>
+          <t>wing_components_comp2_Y (N)</t>
         </is>
       </c>
       <c r="B120" t="n">
-        <v>0.1901605316065426</v>
+        <v>0</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>wing_components_comp2_oswald</t>
+          <t>wing_components_comp2_l_b</t>
         </is>
       </c>
       <c r="B121" t="n">
-        <v>0.8106853777008906</v>
+        <v>4.607859233063394e-19</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>wing_components_comp3_L (N)</t>
+          <t>wing_components_comp2_m_b</t>
         </is>
       </c>
       <c r="B122" t="n">
-        <v>-2.710505431213761e-20</v>
+        <v>-0.03964930383101905</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>wing_components_comp3_D (N)</t>
+          <t>wing_components_comp2_n_b</t>
         </is>
       </c>
       <c r="B123" t="n">
-        <v>0.001214685578902999</v>
+        <v>3.218725199566341e-20</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>wing_components_comp3_Y (N)</t>
+          <t>wing_components_comp2_span_eff (m)</t>
         </is>
       </c>
       <c r="B124" t="n">
-        <v>3.847629485179784e-17</v>
+        <v>0.1901606678026856</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>wing_components_comp3_l_b</t>
+          <t>wing_components_comp2_oswald</t>
         </is>
       </c>
       <c r="B125" t="n">
-        <v>1.255088091123217e-18</v>
+        <v>0.8106853777008906</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>wing_components_comp3_m_b</t>
+          <t>wing_components_comp3_L (N)</t>
         </is>
       </c>
       <c r="B126" t="n">
-        <v>-9.620038079883495e-05</v>
+        <v>8.131516293641283e-20</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>wing_components_comp3_n_b</t>
+          <t>wing_components_comp3_D (N)</t>
         </is>
       </c>
       <c r="B127" t="n">
-        <v>-2.466629380484286e-17</v>
+        <v>0.001214686697835623</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>wing_components_comp3_span_eff (m)</t>
+          <t>wing_components_comp3_Y (N)</t>
         </is>
       </c>
       <c r="B128" t="n">
-        <v>0.07145088433007531</v>
+        <v>4.424779351762667e-17</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>wing_components_comp3_oswald</t>
+          <t>wing_components_comp3_l_b</t>
         </is>
       </c>
       <c r="B129" t="n">
-        <v>0.8232692748986458</v>
+        <v>1.433164975032449e-18</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>fuselage_components_comp1_L (N)</t>
+          <t>wing_components_comp3_m_b</t>
         </is>
       </c>
       <c r="B130" t="n">
-        <v>0.001687462744819375</v>
+        <v>-9.620017666279131e-05</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>fuselage_components_comp1_D (N)</t>
+          <t>wing_components_comp3_n_b</t>
         </is>
       </c>
       <c r="B131" t="n">
-        <v>0.001327473498832547</v>
+        <v>-2.83084317442758e-17</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>fuselage_components_comp1_Y (N)</t>
+          <t>wing_components_comp3_span_eff (m)</t>
         </is>
       </c>
       <c r="B132" t="n">
-        <v>0</v>
+        <v>0.07145092947298221</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>fuselage_components_comp1_l_b</t>
+          <t>wing_components_comp3_oswald</t>
         </is>
       </c>
       <c r="B133" t="n">
-        <v>2.586811642531295e-21</v>
+        <v>0.8232692748986458</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>fuselage_components_comp1_m_b</t>
+          <t>fuselage_components_comp1_L (N)</t>
         </is>
       </c>
       <c r="B134" t="n">
-        <v>-0.0004958407535257094</v>
+        <v>0.001687459512573406</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>fuselage_components_comp1_n_b</t>
+          <t>fuselage_components_comp1_D (N)</t>
         </is>
       </c>
       <c r="B135" t="n">
-        <v>-1.386513622231565e-21</v>
+        <v>0.00132747144246971</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>fuselage_components_comp1_span_eff (m)</t>
+          <t>fuselage_components_comp1_Y (N)</t>
         </is>
       </c>
       <c r="B136" t="n">
-        <v>0.004055451774444796</v>
+        <v>0</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>fuselage_components_comp1_oswald</t>
+          <t>fuselage_components_comp1_l_b</t>
         </is>
       </c>
       <c r="B137" t="n">
-        <v>0.95</v>
+        <v>1.372821843636459e-20</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>aero_D_profile</t>
+          <t>fuselage_components_comp1_m_b</t>
         </is>
       </c>
       <c r="B138" t="n">
-        <v>0.07684185087228773</v>
+        <v>-0.0004958388830935519</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>aero_D_induced</t>
+          <t>fuselage_components_comp1_n_b</t>
         </is>
       </c>
       <c r="B139" t="n">
-        <v>0.1375954607743183</v>
+        <v>-7.358235789878711e-21</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>aero_CLa</t>
+          <t>fuselage_components_comp1_span_eff (m)</t>
         </is>
       </c>
       <c r="B140" t="n">
-        <v>4.064859259811374</v>
+        <v>0.004055451774444796</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>aero_CDa</t>
+          <t>fuselage_components_comp1_oswald</t>
         </is>
       </c>
       <c r="B141" t="n">
-        <v>0.6767862506314274</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>aero_CYa</t>
+          <t>aero_D_profile</t>
         </is>
       </c>
       <c r="B142" t="n">
-        <v>4.778943697127297e-13</v>
+        <v>0.07684184335256521</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>aero_Cla</t>
+          <t>aero_D_induced</t>
         </is>
       </c>
       <c r="B143" t="n">
-        <v>4.672255556381167e-12</v>
+        <v>0.137595445237259</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>aero_Cma</t>
+          <t>aero_CLa</t>
         </is>
       </c>
       <c r="B144" t="n">
-        <v>-0.1625946708973857</v>
+        <v>4.064860340500243</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>aero_Cna</t>
+          <t>aero_CDa</t>
         </is>
       </c>
       <c r="B145" t="n">
-        <v>1.133709065351193e-12</v>
+        <v>0.6767865219637521</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>aero_x_np</t>
+          <t>aero_CYa</t>
         </is>
       </c>
       <c r="B146" t="n">
-        <v>0.03238117803743063</v>
+        <v>-9.111397247937444e-22</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>aero_CLb</t>
+          <t>aero_Cla</t>
         </is>
       </c>
       <c r="B147" t="n">
-        <v>-5.506163542330915e-06</v>
+        <v>4.294411288492044e-15</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>aero_CDb</t>
+          <t>aero_Cma</t>
         </is>
       </c>
       <c r="B148" t="n">
-        <v>-6.06345715306227e-07</v>
+        <v>-0.1625947182930564</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>aero_CYb</t>
+          <t>aero_Cna</t>
         </is>
       </c>
       <c r="B149" t="n">
-        <v>0.1356589143117148</v>
+        <v>1.341941148725146e-16</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>aero_Clb</t>
+          <t>aero_x_np</t>
         </is>
       </c>
       <c r="B150" t="n">
-        <v>-0.02500007760572317</v>
+        <v>0.03238118625267943</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>aero_Cmb</t>
+          <t>aero_CLb</t>
         </is>
       </c>
       <c r="B151" t="n">
-        <v>7.542020001801948e-07</v>
+        <v>-5.506278042299447e-06</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>aero_Cnb</t>
+          <t>aero_CDb</t>
         </is>
       </c>
       <c r="B152" t="n">
-        <v>0.02026732680355855</v>
+        <v>-6.063751354370306e-07</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>aero_x_np_lateral</t>
+          <t>aero_CYb</t>
         </is>
       </c>
       <c r="B153" t="n">
-        <v>-0.09200479311624762</v>
+        <v>0.1356588761107938</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>aero_CLp</t>
+          <t>aero_Clb</t>
         </is>
       </c>
       <c r="B154" t="n">
-        <v>-0.007946218976373485</v>
+        <v>-0.02500007761348012</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>aero_CDp</t>
+          <t>aero_Cmb</t>
         </is>
       </c>
       <c r="B155" t="n">
-        <v>-0.001728879209142442</v>
+        <v>7.541831634295015e-07</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>aero_CYp</t>
+          <t>aero_Cnb</t>
         </is>
       </c>
       <c r="B156" t="n">
-        <v>-0.07824093178048834</v>
+        <v>0.020267310265257</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>aero_Clp</t>
+          <t>aero_x_np_lateral</t>
         </is>
       </c>
       <c r="B157" t="n">
-        <v>-0.6483471936163293</v>
+        <v>-0.09200469489551635</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>aero_Cmp</t>
+          <t>aero_CLp</t>
         </is>
       </c>
       <c r="B158" t="n">
-        <v>-0.0003117836891300668</v>
+        <v>-0.007946216506571346</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>aero_Cnp</t>
+          <t>aero_CDp</t>
         </is>
       </c>
       <c r="B159" t="n">
-        <v>-0.2730784457068493</v>
+        <v>-0.001728879776619063</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>aero_CLq</t>
+          <t>aero_CYp</t>
         </is>
       </c>
       <c r="B160" t="n">
-        <v>0.3851217171442211</v>
+        <v>-0.07824093524226554</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>aero_CDq</t>
+          <t>aero_Clp</t>
         </is>
       </c>
       <c r="B161" t="n">
-        <v>0.5315076374927813</v>
+        <v>-0.6483472779705023</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>aero_CYq</t>
+          <t>aero_Cmp</t>
         </is>
       </c>
       <c r="B162" t="n">
-        <v>-4.001922917485146e-15</v>
+        <v>-0.0003117826050916667</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>aero_Clq</t>
+          <t>aero_Cnp</t>
         </is>
       </c>
       <c r="B163" t="n">
-        <v>-4.796664531084883e-14</v>
+        <v>-0.2730784561490696</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>aero_Cmq</t>
+          <t>aero_CLq</t>
         </is>
       </c>
       <c r="B164" t="n">
-        <v>-10.53214533779856</v>
+        <v>0.3851219621295864</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>aero_Cnq</t>
+          <t>aero_CDq</t>
         </is>
       </c>
       <c r="B165" t="n">
-        <v>-9.633464440542662e-15</v>
+        <v>0.5315074244337802</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>aero_CLr</t>
+          <t>aero_CYq</t>
         </is>
       </c>
       <c r="B166" t="n">
-        <v>-0.000138354317336109</v>
+        <v>5.673802473961533e-17</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>aero_CDr</t>
+          <t>aero_Clq</t>
         </is>
       </c>
       <c r="B167" t="n">
-        <v>-3.183322809519051e-05</v>
+        <v>4.910880792124132e-15</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>aero_CYr</t>
+          <t>aero_Cmq</t>
         </is>
       </c>
       <c r="B168" t="n">
-        <v>0.08964988694207224</v>
+        <v>-10.5321304560436</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>aero_Clr</t>
+          <t>aero_Cnq</t>
         </is>
       </c>
       <c r="B169" t="n">
-        <v>0.2217406785380238</v>
+        <v>-3.636043161460577e-17</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>aero_Cmr</t>
+          <t>aero_CLr</t>
         </is>
       </c>
       <c r="B170" t="n">
-        <v>-9.254742128052122e-05</v>
+        <v>-0.0001383543133393061</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
+          <t>aero_CDr</t>
+        </is>
+      </c>
+      <c r="B171" t="n">
+        <v>-3.183309975340887e-05</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>aero_CYr</t>
+        </is>
+      </c>
+      <c r="B172" t="n">
+        <v>0.08964985658511813</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>aero_Clr</t>
+        </is>
+      </c>
+      <c r="B173" t="n">
+        <v>0.22174064668748</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>aero_Cmr</t>
+        </is>
+      </c>
+      <c r="B174" t="n">
+        <v>-9.254728702718008e-05</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
           <t>aero_Cnr</t>
         </is>
       </c>
-      <c r="B171" t="n">
-        <v>-0.04708441779698663</v>
+      <c r="B175" t="n">
+        <v>-0.04708432312542851</v>
       </c>
     </row>
   </sheetData>

</xml_diff>